<commit_message>
Segragated each battery data from 3 battery hours Bytebeam data and stored it in a separate excel file!
</commit_message>
<xml_diff>
--- a/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V4/D11_03_2024/B3_B03_13.15_15.30/analysis_B3_B03_13.15_15.30.xlsx
+++ b/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V4/D11_03_2024/B3_B03_13.15_15.30/analysis_B3_B03_13.15_15.30.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
@@ -491,13 +491,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Total distance covered (in kilometers)</t>
+          <t>Total distance covered (km)</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -507,7 +507,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WH/KM</t>
+          <t>Total energy consumption(WH/KM)</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -517,7 +517,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total SOC consumed</t>
+          <t>Total SOC consumed(%)</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -540,7 +540,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Peak Power</t>
+          <t>Peak Power(kW)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -550,7 +550,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Average Power</t>
+          <t>Average Power(kW)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -560,7 +560,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Total Energy Regenerated</t>
+          <t>Total Energy Regenerated(kWh)</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -570,7 +570,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Regenerative Effectiveness</t>
+          <t>Regenerative Effectiveness(kWh)</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -580,27 +580,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lowest Cell Voltage</t>
+          <t>Highest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.985</v>
+        <v>3.339</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Highest Cell Voltage</t>
+          <t>Lowest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.339</v>
+        <v>2.985</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Difference in Cell Voltage</t>
+          <t>Difference in Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -610,7 +610,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Minimum Temperature</t>
+          <t>Minimum Temperature(C)</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -620,7 +620,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Maximum Temperature</t>
+          <t>Maximum Temperature(C)</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -630,17 +630,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Difference in Temperature</t>
+          <t>Difference in Temperature(C)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v/>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Maximum Fet Temperature</t>
+          <t>Maximum Fet Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -650,7 +650,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maximum Afe Temperature</t>
+          <t>Maximum Afe Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -660,7 +660,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Maximum PCB Temperature</t>
+          <t>Maximum PCB Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -670,7 +670,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Maximum MCU Temperature</t>
+          <t>Maximum MCU Temperature(C)</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -680,7 +680,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Maximum Motor Temperature</t>
+          <t>Maximum Motor Temperature(C)</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -690,7 +690,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Abnormal Motor Temperature Detected</t>
+          <t>Abnormal Motor Temperature Detected(C)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -700,7 +700,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lowest cell temp</t>
+          <t>highest cell temp(C)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -710,7 +710,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>highest cell temp</t>
+          <t>lowest cell temp(C)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -720,7 +720,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC</t>
+          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC(C)</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -730,107 +730,107 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Maximum BMS Temperature in C</t>
+          <t>Battery Voltage(V)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Battery Voltage</t>
+          <t>Total energy charged(kWh)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5.5</v>
+        <v>1.970930148611111</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Total energy charged in kWh</t>
+          <t>Electricity consumption units(kW)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1970930148611111</v>
+        <v>6.687194293836812e-08</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Electricity consumption units in kW</t>
+          <t>Idling time percentage</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>6.687194293836812e-09</v>
+        <v>18.29305715381665</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Idling time percentage</t>
+          <t>Time spent in 0-10 km/h</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17.45556834164429</v>
+        <v>4.760260836210203</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Time spent in 0-10 km/h</t>
+          <t>Time spent in 10-20 km/h</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>22.21582917785449</v>
+        <v>1.663470144482803</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Time spent in 10-20 km/h</t>
+          <t>Time spent in 20-30 km/h</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1.664748753356348</v>
+        <v>3.11724843370413</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Time spent in 20-30 km/h</t>
+          <t>Time spent in 30-40 km/h</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3.122362869198312</v>
+        <v>41.70950006393044</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Time spent in 30-40 km/h</t>
+          <t>Time spent in 40-50 km/h</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>41.71205728167753</v>
+        <v>28.17286791970336</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Time spent in 40-50 km/h</t>
+          <t>Time spent in 50-60 km/h</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>30.44751310574095</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Time spent in 50-60 km/h</t>
+          <t>Time spent in 60-70 km/h</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -840,10 +840,20 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Time spent in 60-70 km/h</t>
+          <t>Time spent in 70-80 km/h</t>
         </is>
       </c>
       <c r="B42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Time spent in 80-90 km/h</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made changes with regenerative effectiveness, Rectified the anomaly in the Total SOC consumed
</commit_message>
<xml_diff>
--- a/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V4/D11_03_2024/B3_B03_13.15_15.30/analysis_B3_B03_13.15_15.30.xlsx
+++ b/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V4/D11_03_2024/B3_B03_13.15_15.30/analysis_B3_B03_13.15_15.30.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
@@ -491,13 +491,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Total distance covered (in kilometers)</t>
+          <t>Total distance covered (km)</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -507,7 +507,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WH/KM</t>
+          <t>Total energy consumption(WH/KM)</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -517,7 +517,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total SOC consumed</t>
+          <t>Total SOC consumed(%)</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -540,7 +540,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Peak Power</t>
+          <t>Peak Power(kW)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -550,7 +550,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Average Power</t>
+          <t>Average Power(kW)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -560,7 +560,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Total Energy Regenerated</t>
+          <t>Total Energy Regenerated(kWh)</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -570,37 +570,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Regenerative Effectiveness</t>
+          <t>Regenerative Effectiveness(%)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.201109951715442</v>
+        <v>1.201109951715442</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lowest Cell Voltage</t>
+          <t>Highest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2.985</v>
+        <v>3.339</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Highest Cell Voltage</t>
+          <t>Lowest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.339</v>
+        <v>2.985</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Difference in Cell Voltage</t>
+          <t>Difference in Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -610,7 +610,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Minimum Temperature</t>
+          <t>Minimum Temperature(C)</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -620,7 +620,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Maximum Temperature</t>
+          <t>Maximum Temperature(C)</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -630,17 +630,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Difference in Temperature</t>
+          <t>Difference in Temperature(C)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v/>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Maximum Fet Temperature</t>
+          <t>Maximum Fet Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -650,7 +650,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maximum Afe Temperature</t>
+          <t>Maximum Afe Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -660,7 +660,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Maximum PCB Temperature</t>
+          <t>Maximum PCB Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -670,7 +670,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Maximum MCU Temperature</t>
+          <t>Maximum MCU Temperature(C)</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -680,7 +680,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Maximum Motor Temperature</t>
+          <t>Maximum Motor Temperature(C)</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -690,7 +690,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Abnormal Motor Temperature Detected</t>
+          <t>Abnormal Motor Temperature Detected(C)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -700,7 +700,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lowest cell temp</t>
+          <t>highest cell temp(C)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -710,7 +710,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>highest cell temp</t>
+          <t>lowest cell temp(C)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -720,7 +720,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC</t>
+          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC(C)</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -730,107 +730,107 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Maximum BMS Temperature in C</t>
+          <t>Battery Voltage(V)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Battery Voltage</t>
+          <t>Total energy charged(kWh)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5.5</v>
+        <v>1.970930148611111</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Total energy charged in kWh</t>
+          <t>Electricity consumption units(kW)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1970930148611111</v>
+        <v>6.687194293836812e-08</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Electricity consumption units in kW</t>
+          <t>Idling time percentage</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>6.687194293836812e-09</v>
+        <v>18.29305715381665</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Idling time percentage</t>
+          <t>Time spent in 0-10 km/h</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17.45556834164429</v>
+        <v>4.760260836210203</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Time spent in 0-10 km/h</t>
+          <t>Time spent in 10-20 km/h</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>22.21582917785449</v>
+        <v>1.663470144482803</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Time spent in 10-20 km/h</t>
+          <t>Time spent in 20-30 km/h</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1.664748753356348</v>
+        <v>3.11724843370413</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Time spent in 20-30 km/h</t>
+          <t>Time spent in 30-40 km/h</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3.122362869198312</v>
+        <v>41.70950006393044</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Time spent in 30-40 km/h</t>
+          <t>Time spent in 40-50 km/h</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>41.71205728167753</v>
+        <v>28.17286791970336</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Time spent in 40-50 km/h</t>
+          <t>Time spent in 50-60 km/h</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>30.44751310574095</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Time spent in 50-60 km/h</t>
+          <t>Time spent in 60-70 km/h</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -840,10 +840,20 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Time spent in 60-70 km/h</t>
+          <t>Time spent in 70-80 km/h</t>
         </is>
       </c>
       <c r="B42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Time spent in 80-90 km/h</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>